<commit_message>
Updated example to better illustrate encodefrom
Merges crime data set with sysuse census data set after encoding the state variables
</commit_message>
<xml_diff>
--- a/example/input/variables.xlsx
+++ b/example/input/variables.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alicia\Desktop\rename-and-encode-master\example\input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="15465"/>
   </bookViews>
   <sheets>
-    <sheet name="census" sheetId="1" r:id="rId1"/>
+    <sheet name="crime" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,156 +25,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>variable</t>
   </si>
   <si>
-    <t>black</t>
-  </si>
-  <si>
-    <t>white</t>
-  </si>
-  <si>
-    <t>pop</t>
-  </si>
-  <si>
     <t>label</t>
   </si>
   <si>
-    <t>asian pacific</t>
-  </si>
-  <si>
-    <t>native american</t>
-  </si>
-  <si>
-    <t>other race</t>
-  </si>
-  <si>
-    <t>total population</t>
-  </si>
-  <si>
-    <t>census_1990</t>
-  </si>
-  <si>
-    <t>P145A001</t>
-  </si>
-  <si>
-    <r>
-      <t>P145</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>001</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>P145C</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>001</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>P145F</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>001</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P001001</t>
-  </si>
-  <si>
-    <t>census_2000_lf</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>areakey</t>
-  </si>
-  <si>
-    <t>tract number</t>
-  </si>
-  <si>
-    <t>asian</t>
-  </si>
-  <si>
-    <t>pacific</t>
-  </si>
-  <si>
-    <t>P145D001</t>
-  </si>
-  <si>
-    <t>P145E001</t>
-  </si>
-  <si>
-    <t>popaspac</t>
-  </si>
-  <si>
-    <t>popblack</t>
-  </si>
-  <si>
-    <t>popnatam</t>
-  </si>
-  <si>
-    <t>popother</t>
-  </si>
-  <si>
-    <t>popwhite</t>
-  </si>
-  <si>
-    <t>totpop90</t>
-  </si>
-  <si>
-    <t>race_asian</t>
-  </si>
-  <si>
-    <t>race_pac</t>
-  </si>
-  <si>
-    <t>pop_aspac</t>
-  </si>
-  <si>
-    <t>pop_black</t>
-  </si>
-  <si>
-    <t>pop_natam</t>
-  </si>
-  <si>
-    <t>pop_other</t>
-  </si>
-  <si>
-    <t>pop_white</t>
+    <t>crime_rates</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>violentcrimerate</t>
+  </si>
+  <si>
+    <t>violent</t>
+  </si>
+  <si>
+    <t>murder</t>
+  </si>
+  <si>
+    <t>murderandnonnegligentmanslaughte</t>
+  </si>
+  <si>
+    <t>Violent crime rate, per 100,000</t>
+  </si>
+  <si>
+    <t>Murder and nonnegligent manslaughter rate, per 100,000</t>
+  </si>
+  <si>
+    <t>rape</t>
+  </si>
+  <si>
+    <t>legacyraperate1</t>
+  </si>
+  <si>
+    <t>Legacy rape rate, per 100,000</t>
+  </si>
+  <si>
+    <t>propertycrimerate</t>
+  </si>
+  <si>
+    <t>Property crime rate, per 100,000</t>
+  </si>
+  <si>
+    <t>property</t>
+  </si>
+  <si>
+    <t>burglaryrate</t>
+  </si>
+  <si>
+    <t>Burglary rate, per 100,000</t>
+  </si>
+  <si>
+    <t>burglary</t>
+  </si>
+  <si>
+    <t>larcenytheftrate</t>
+  </si>
+  <si>
+    <t>Larceny theft rate, per 100,000</t>
+  </si>
+  <si>
+    <t>larceny</t>
+  </si>
+  <si>
+    <t>motorvehicletheftrate</t>
+  </si>
+  <si>
+    <t>Motor vehicle theft rate, per 100,000</t>
+  </si>
+  <si>
+    <t>vehicle</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -179,11 +119,6 @@
       <name val="돋움"/>
       <family val="3"/>
       <charset val="129"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -206,13 +141,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,7 +416,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -493,149 +424,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
         <v>23</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -658,9 +556,9 @@
       <selection activeCell="A57" sqref="A57:A71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="2"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
   </cols>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>